<commit_message>
grafico e menu 1
Foi feito o gráfico, titulo e menu no dashboard
</commit_message>
<xml_diff>
--- a/dashboard_xbox_sales.xlsx
+++ b/dashboard_xbox_sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DIO\DIO-Vendas-do-Xbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29AF995-3DE6-40D8-8A20-7AC5533F482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D732D19-83D6-4C11-BA2F-CB1366E4BFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
     <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,22 @@
     <sheet name="C̳álculos" sheetId="3" r:id="rId3"/>
     <sheet name="D̳ashboard" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="SegmentaçãodeDados_Subscription_Type">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -33,8 +44,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="320">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1089,15 +1098,18 @@
   <si>
     <t>Total Geral</t>
   </si>
+  <si>
+    <t>XBOX GAME PASS SUBSCRITIONS SALES</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,6 +1153,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF2AE6B1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1198,7 +1217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1215,6 +1234,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF22C55E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1222,7 +1250,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1252,6 +1280,7 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1259,7 +1288,66 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF2AE6B1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1309,30 +1397,2740 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="SlicerStyleLight6 2" pivot="0" table="0" count="10" xr9:uid="{14279B14-3B4E-4DF9-8110-D0080E74140C}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF2AE6B1"/>
+      <color rgb="FF5BF6A8"/>
       <color rgb="FF22C55E"/>
       <color rgb="FFE8E6E9"/>
-      <color rgb="FF5BF6A8"/>
       <color rgb="FF000000"/>
       <color rgb="FFE0E0E0"/>
       <color rgb="FFEDEDED"/>
       <color rgb="FFF7F8FC"/>
-      <color rgb="FF2AE6B1"/>
       <color rgb="FF9BC848"/>
       <color rgb="FFE70011"/>
     </mruColors>
   </colors>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
+      <x14:dxfs count="32">
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+      </x14:dxfs>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1">
+        <x14:slicerStyle name="SlicerStyleLight6 2">
+          <x14:slicerStyleElements>
+            <x14:slicerStyleElement type="unselectedItemWithData" dxfId="7"/>
+            <x14:slicerStyleElement type="unselectedItemWithNoData" dxfId="6"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="5"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="4"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithData" dxfId="3"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithData" dxfId="2"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithNoData" dxfId="1"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="0"/>
+          </x14:slicerStyleElements>
+        </x14:slicerStyle>
+      </x14:slicerStyles>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dashboard_xbox_sales.xlsx]C̳álculos!Tabela dinâmica1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>C̳álculos!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5BF6A8"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>C̳álculos!$B$13:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>C̳álculos!$C$13:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE7C-4E69-8EEE-96FA5565D736}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="136401296"/>
+        <c:axId val="136399216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="136401296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="136399216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="136399216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="136401296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dashboard_xbox_sales.xlsx]C̳álculos!Tabela dinâmica1</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>C̳álculos!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5BF6A8"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>C̳álculos!$B$13:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>C̳álculos!$C$13:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD02-49A8-985C-B4A6592C8EC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="136401296"/>
+        <c:axId val="136399216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="136401296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="136399216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="136399216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="136401296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2072,6 +4870,363 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1014412</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1452562</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C31DBE3-FCBE-42E1-B232-172825399995}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Subscription Type">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E0DF54-F4DF-4AAB-9E6D-6E9939F7FA9F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Subscription Type"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6105525" y="2295525"/>
+              <a:ext cx="2076450" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142873</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1262062</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>261936</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C860A6-1DE0-43E6-8AE9-A1A17B283A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="6560" t="17103" r="71574" b="19371"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="547687" y="321467"/>
+          <a:ext cx="714375" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>392906</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Agrupar 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68C129F-59AF-49AD-963B-B801145A6497}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2583657" y="1393031"/>
+          <a:ext cx="5048249" cy="3083719"/>
+          <a:chOff x="5143500" y="1785937"/>
+          <a:chExt cx="5048250" cy="3083719"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Retângulo: Cantos Arredondados 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32857F68-3BAC-436F-ABF4-EF65D0C690B8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5143500" y="1785937"/>
+            <a:ext cx="5048250" cy="3083719"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 4698"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Gráfico 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5758FA93-B434-4E32-8E8D-84DEFAE385CF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="5405436" y="1952626"/>
+          <a:ext cx="4572001" cy="2743200"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>78582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2076450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>150019</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Subscription Type 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7399B383-BBED-459C-A26C-000F288422D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Subscription Type 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1459707"/>
+              <a:ext cx="2076450" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2130,7 +5285,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1162036948"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -6567,7 +9722,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EC8D6D2-BFCC-48E6-989A-4B46A9CE0253}" name="Tabela dinâmica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EC8D6D2-BFCC-48E6-989A-4B46A9CE0253}" name="Tabela dinâmica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B12:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -6615,16 +9770,48 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="0" hier="-1"/>
+    <pageField fld="6" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Total Value" fld="12" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -6637,8 +9824,37 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Subscription_Type" xr10:uid="{0D8AF5E2-2E6B-4BB8-BAC2-37FA7F95A8FD}" sourceName="Subscription Type">
+  <pivotTables>
+    <pivotTable tabId="3" name="Tabela dinâmica1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1162036948">
+      <items count="3">
+        <i x="1"/>
+        <i x="0"/>
+        <i x="2" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Subscription Type" xr10:uid="{2577FA2C-726B-4A41-A454-37E836B311B6}" cache="SegmentaçãodeDados_Subscription_Type" caption="Subscription Type" style="SlicerStyleLight6" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Subscription Type 1" xr10:uid="{FF8009D7-D4F7-449F-BFC9-CD4FABB74537}" cache="SegmentaçãodeDados_Subscription_Type" caption="Subscription Type" style="SlicerStyleLight6 2" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="7">
       <filters>
@@ -6647,19 +9863,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="9" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="6" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="3" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="20" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="17" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="15" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="14" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="13" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6988,7 +10204,7 @@
   <dimension ref="B3:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -19333,8 +22549,8 @@
   </sheetPr>
   <dimension ref="B3:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -19377,7 +22593,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -19393,7 +22609,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="15">
-        <v>217</v>
+        <v>806</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -19401,7 +22617,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="15">
-        <v>1537</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -19409,7 +22625,7 @@
         <v>318</v>
       </c>
       <c r="C15" s="15">
-        <v>1754</v>
+        <v>2308</v>
       </c>
     </row>
   </sheetData>
@@ -19418,32 +22634,556 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A2:Q168"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="28" style="5" customWidth="1"/>
     <col min="2" max="2" width="3.625" customWidth="1"/>
     <col min="12" max="12" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="39" customHeight="1"/>
-    <row r="3" ht="8.25" customHeight="1"/>
-    <row r="4" ht="7.5" customHeight="1"/>
-    <row r="5" ht="10.5" customHeight="1"/>
-    <row r="6" ht="9.75" customHeight="1"/>
-    <row r="7" ht="33" customHeight="1"/>
+    <row r="2" spans="1:17" ht="39" customHeight="1" thickBot="1">
+      <c r="C2" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" ht="39" customHeight="1" thickTop="1"/>
+    <row r="4" spans="1:17" s="7" customFormat="1" ht="8.25" customHeight="1">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" s="7" customFormat="1" ht="7.5" customHeight="1">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" s="7" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" s="7" customFormat="1" ht="9.75" customHeight="1">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" s="7" customFormat="1" ht="33" customHeight="1">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" s="7" customFormat="1">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" s="7" customFormat="1">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" s="7" customFormat="1">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" s="7" customFormat="1">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" s="7" customFormat="1">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" s="7" customFormat="1">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" s="7" customFormat="1">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" s="7" customFormat="1">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" s="7" customFormat="1">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" s="7" customFormat="1">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:1" s="7" customFormat="1">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" s="7" customFormat="1">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" s="7" customFormat="1">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:1" s="7" customFormat="1">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:1" s="7" customFormat="1">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:1" s="7" customFormat="1">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:1" s="7" customFormat="1">
+      <c r="A25" s="5"/>
+    </row>
+    <row r="26" spans="1:1" s="7" customFormat="1">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:1" s="7" customFormat="1">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:1" s="7" customFormat="1">
+      <c r="A28" s="5"/>
+    </row>
+    <row r="29" spans="1:1" s="7" customFormat="1">
+      <c r="A29" s="5"/>
+    </row>
+    <row r="30" spans="1:1" s="7" customFormat="1">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:1" s="7" customFormat="1">
+      <c r="A31" s="5"/>
+    </row>
+    <row r="32" spans="1:1" s="7" customFormat="1">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" s="7" customFormat="1">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1" s="7" customFormat="1">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:1" s="7" customFormat="1">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:1" s="7" customFormat="1">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:1" s="7" customFormat="1">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:1" s="7" customFormat="1">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:1" s="7" customFormat="1">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:1" s="7" customFormat="1">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:1" s="7" customFormat="1">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" spans="1:1" s="7" customFormat="1">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:1" s="7" customFormat="1">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:1" s="7" customFormat="1">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:1" s="7" customFormat="1">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:1" s="7" customFormat="1">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:1" s="7" customFormat="1">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:1" s="7" customFormat="1">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:1" s="7" customFormat="1">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" s="7" customFormat="1">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:1" s="7" customFormat="1">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" spans="1:1" s="7" customFormat="1">
+      <c r="A52" s="5"/>
+    </row>
+    <row r="53" spans="1:1" s="7" customFormat="1">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" spans="1:1" s="7" customFormat="1">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" spans="1:1" s="7" customFormat="1">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" spans="1:1" s="7" customFormat="1">
+      <c r="A56" s="5"/>
+    </row>
+    <row r="57" spans="1:1" s="7" customFormat="1">
+      <c r="A57" s="5"/>
+    </row>
+    <row r="58" spans="1:1" s="7" customFormat="1">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:1" s="7" customFormat="1">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" spans="1:1" s="7" customFormat="1">
+      <c r="A60" s="5"/>
+    </row>
+    <row r="61" spans="1:1" s="7" customFormat="1">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:1" s="7" customFormat="1">
+      <c r="A62" s="5"/>
+    </row>
+    <row r="63" spans="1:1" s="7" customFormat="1">
+      <c r="A63" s="5"/>
+    </row>
+    <row r="64" spans="1:1" s="7" customFormat="1">
+      <c r="A64" s="5"/>
+    </row>
+    <row r="65" spans="1:1" s="7" customFormat="1">
+      <c r="A65" s="5"/>
+    </row>
+    <row r="66" spans="1:1" s="7" customFormat="1">
+      <c r="A66" s="5"/>
+    </row>
+    <row r="67" spans="1:1" s="7" customFormat="1">
+      <c r="A67" s="5"/>
+    </row>
+    <row r="68" spans="1:1" s="7" customFormat="1">
+      <c r="A68" s="5"/>
+    </row>
+    <row r="69" spans="1:1" s="7" customFormat="1">
+      <c r="A69" s="5"/>
+    </row>
+    <row r="70" spans="1:1" s="7" customFormat="1">
+      <c r="A70" s="5"/>
+    </row>
+    <row r="71" spans="1:1" s="7" customFormat="1">
+      <c r="A71" s="5"/>
+    </row>
+    <row r="72" spans="1:1" s="7" customFormat="1">
+      <c r="A72" s="5"/>
+    </row>
+    <row r="73" spans="1:1" s="7" customFormat="1">
+      <c r="A73" s="5"/>
+    </row>
+    <row r="74" spans="1:1" s="7" customFormat="1">
+      <c r="A74" s="5"/>
+    </row>
+    <row r="75" spans="1:1" s="7" customFormat="1">
+      <c r="A75" s="5"/>
+    </row>
+    <row r="76" spans="1:1" s="7" customFormat="1">
+      <c r="A76" s="5"/>
+    </row>
+    <row r="77" spans="1:1" s="7" customFormat="1">
+      <c r="A77" s="5"/>
+    </row>
+    <row r="78" spans="1:1" s="7" customFormat="1">
+      <c r="A78" s="5"/>
+    </row>
+    <row r="79" spans="1:1" s="7" customFormat="1">
+      <c r="A79" s="5"/>
+    </row>
+    <row r="80" spans="1:1" s="7" customFormat="1">
+      <c r="A80" s="5"/>
+    </row>
+    <row r="81" spans="1:1" s="7" customFormat="1">
+      <c r="A81" s="5"/>
+    </row>
+    <row r="82" spans="1:1" s="7" customFormat="1">
+      <c r="A82" s="5"/>
+    </row>
+    <row r="83" spans="1:1" s="7" customFormat="1">
+      <c r="A83" s="5"/>
+    </row>
+    <row r="84" spans="1:1" s="7" customFormat="1">
+      <c r="A84" s="5"/>
+    </row>
+    <row r="85" spans="1:1" s="7" customFormat="1">
+      <c r="A85" s="5"/>
+    </row>
+    <row r="86" spans="1:1" s="7" customFormat="1">
+      <c r="A86" s="5"/>
+    </row>
+    <row r="87" spans="1:1" s="7" customFormat="1">
+      <c r="A87" s="5"/>
+    </row>
+    <row r="88" spans="1:1" s="7" customFormat="1">
+      <c r="A88" s="5"/>
+    </row>
+    <row r="89" spans="1:1" s="7" customFormat="1">
+      <c r="A89" s="5"/>
+    </row>
+    <row r="90" spans="1:1" s="7" customFormat="1">
+      <c r="A90" s="5"/>
+    </row>
+    <row r="91" spans="1:1" s="7" customFormat="1">
+      <c r="A91" s="5"/>
+    </row>
+    <row r="92" spans="1:1" s="7" customFormat="1">
+      <c r="A92" s="5"/>
+    </row>
+    <row r="93" spans="1:1" s="7" customFormat="1">
+      <c r="A93" s="5"/>
+    </row>
+    <row r="94" spans="1:1" s="7" customFormat="1">
+      <c r="A94" s="5"/>
+    </row>
+    <row r="95" spans="1:1" s="7" customFormat="1">
+      <c r="A95" s="5"/>
+    </row>
+    <row r="96" spans="1:1" s="7" customFormat="1">
+      <c r="A96" s="5"/>
+    </row>
+    <row r="97" spans="1:1" s="7" customFormat="1">
+      <c r="A97" s="5"/>
+    </row>
+    <row r="98" spans="1:1" s="7" customFormat="1">
+      <c r="A98" s="5"/>
+    </row>
+    <row r="99" spans="1:1" s="7" customFormat="1">
+      <c r="A99" s="5"/>
+    </row>
+    <row r="100" spans="1:1" s="7" customFormat="1">
+      <c r="A100" s="5"/>
+    </row>
+    <row r="101" spans="1:1" s="7" customFormat="1">
+      <c r="A101" s="5"/>
+    </row>
+    <row r="102" spans="1:1" s="7" customFormat="1">
+      <c r="A102" s="5"/>
+    </row>
+    <row r="103" spans="1:1" s="7" customFormat="1">
+      <c r="A103" s="5"/>
+    </row>
+    <row r="104" spans="1:1" s="7" customFormat="1">
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:1" s="7" customFormat="1">
+      <c r="A105" s="5"/>
+    </row>
+    <row r="106" spans="1:1" s="7" customFormat="1">
+      <c r="A106" s="5"/>
+    </row>
+    <row r="107" spans="1:1" s="7" customFormat="1">
+      <c r="A107" s="5"/>
+    </row>
+    <row r="108" spans="1:1" s="7" customFormat="1">
+      <c r="A108" s="5"/>
+    </row>
+    <row r="109" spans="1:1" s="7" customFormat="1">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:1" s="7" customFormat="1">
+      <c r="A110" s="5"/>
+    </row>
+    <row r="111" spans="1:1" s="7" customFormat="1">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:1" s="7" customFormat="1">
+      <c r="A112" s="5"/>
+    </row>
+    <row r="113" spans="1:1" s="7" customFormat="1">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="114" spans="1:1" s="7" customFormat="1">
+      <c r="A114" s="5"/>
+    </row>
+    <row r="115" spans="1:1" s="7" customFormat="1">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:1" s="7" customFormat="1">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:1" s="7" customFormat="1">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:1" s="7" customFormat="1">
+      <c r="A118" s="5"/>
+    </row>
+    <row r="119" spans="1:1" s="7" customFormat="1">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="120" spans="1:1" s="7" customFormat="1">
+      <c r="A120" s="5"/>
+    </row>
+    <row r="121" spans="1:1" s="7" customFormat="1">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:1" s="7" customFormat="1">
+      <c r="A122" s="5"/>
+    </row>
+    <row r="123" spans="1:1" s="7" customFormat="1">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:1" s="7" customFormat="1">
+      <c r="A124" s="5"/>
+    </row>
+    <row r="125" spans="1:1" s="7" customFormat="1">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:1" s="7" customFormat="1">
+      <c r="A126" s="5"/>
+    </row>
+    <row r="127" spans="1:1" s="7" customFormat="1">
+      <c r="A127" s="5"/>
+    </row>
+    <row r="128" spans="1:1" s="7" customFormat="1">
+      <c r="A128" s="5"/>
+    </row>
+    <row r="129" spans="1:1" s="7" customFormat="1">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:1" s="7" customFormat="1">
+      <c r="A130" s="5"/>
+    </row>
+    <row r="131" spans="1:1" s="7" customFormat="1">
+      <c r="A131" s="5"/>
+    </row>
+    <row r="132" spans="1:1" s="7" customFormat="1">
+      <c r="A132" s="5"/>
+    </row>
+    <row r="133" spans="1:1" s="7" customFormat="1">
+      <c r="A133" s="5"/>
+    </row>
+    <row r="134" spans="1:1" s="7" customFormat="1">
+      <c r="A134" s="5"/>
+    </row>
+    <row r="135" spans="1:1" s="7" customFormat="1">
+      <c r="A135" s="5"/>
+    </row>
+    <row r="136" spans="1:1" s="7" customFormat="1">
+      <c r="A136" s="5"/>
+    </row>
+    <row r="137" spans="1:1" s="7" customFormat="1">
+      <c r="A137" s="5"/>
+    </row>
+    <row r="138" spans="1:1" s="7" customFormat="1">
+      <c r="A138" s="5"/>
+    </row>
+    <row r="139" spans="1:1" s="7" customFormat="1">
+      <c r="A139" s="5"/>
+    </row>
+    <row r="140" spans="1:1" s="7" customFormat="1">
+      <c r="A140" s="5"/>
+    </row>
+    <row r="141" spans="1:1" s="7" customFormat="1">
+      <c r="A141" s="5"/>
+    </row>
+    <row r="142" spans="1:1" s="7" customFormat="1">
+      <c r="A142" s="5"/>
+    </row>
+    <row r="143" spans="1:1" s="7" customFormat="1">
+      <c r="A143" s="5"/>
+    </row>
+    <row r="144" spans="1:1" s="7" customFormat="1">
+      <c r="A144" s="5"/>
+    </row>
+    <row r="145" spans="1:1" s="7" customFormat="1">
+      <c r="A145" s="5"/>
+    </row>
+    <row r="146" spans="1:1" s="7" customFormat="1">
+      <c r="A146" s="5"/>
+    </row>
+    <row r="147" spans="1:1" s="7" customFormat="1">
+      <c r="A147" s="5"/>
+    </row>
+    <row r="148" spans="1:1" s="7" customFormat="1">
+      <c r="A148" s="5"/>
+    </row>
+    <row r="149" spans="1:1" s="7" customFormat="1">
+      <c r="A149" s="5"/>
+    </row>
+    <row r="150" spans="1:1" s="7" customFormat="1">
+      <c r="A150" s="5"/>
+    </row>
+    <row r="151" spans="1:1" s="7" customFormat="1">
+      <c r="A151" s="5"/>
+    </row>
+    <row r="152" spans="1:1" s="7" customFormat="1">
+      <c r="A152" s="5"/>
+    </row>
+    <row r="153" spans="1:1" s="7" customFormat="1">
+      <c r="A153" s="5"/>
+    </row>
+    <row r="154" spans="1:1" s="7" customFormat="1">
+      <c r="A154" s="5"/>
+    </row>
+    <row r="155" spans="1:1" s="7" customFormat="1">
+      <c r="A155" s="5"/>
+    </row>
+    <row r="156" spans="1:1" s="7" customFormat="1">
+      <c r="A156" s="5"/>
+    </row>
+    <row r="157" spans="1:1" s="7" customFormat="1">
+      <c r="A157" s="5"/>
+    </row>
+    <row r="158" spans="1:1" s="7" customFormat="1">
+      <c r="A158" s="5"/>
+    </row>
+    <row r="159" spans="1:1" s="7" customFormat="1">
+      <c r="A159" s="5"/>
+    </row>
+    <row r="160" spans="1:1" s="7" customFormat="1">
+      <c r="A160" s="5"/>
+    </row>
+    <row r="161" spans="1:1" s="7" customFormat="1">
+      <c r="A161" s="5"/>
+    </row>
+    <row r="162" spans="1:1" s="7" customFormat="1">
+      <c r="A162" s="5"/>
+    </row>
+    <row r="163" spans="1:1" s="7" customFormat="1">
+      <c r="A163" s="5"/>
+    </row>
+    <row r="164" spans="1:1" s="7" customFormat="1">
+      <c r="A164" s="5"/>
+    </row>
+    <row r="165" spans="1:1" s="7" customFormat="1">
+      <c r="A165" s="5"/>
+    </row>
+    <row r="166" spans="1:1" s="7" customFormat="1">
+      <c r="A166" s="5"/>
+    </row>
+    <row r="167" spans="1:1" s="7" customFormat="1">
+      <c r="A167" s="5"/>
+    </row>
+    <row r="168" spans="1:1" s="7" customFormat="1">
+      <c r="A168" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId2"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Respondendo pergunta 4 e BigNumber2
</commit_message>
<xml_diff>
--- a/dashboard_xbox_sales.xlsx
+++ b/dashboard_xbox_sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DIO\DIO-Vendas-do-Xbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3997B9B0-A4ED-4FBB-8D1D-82F632E764BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163C9D87-F8BE-45C3-8F77-AB9D484C136E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="324">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1106,6 +1106,12 @@
   </si>
   <si>
     <t>Soma de EA Play Season Pass</t>
+  </si>
+  <si>
+    <t>Pergunta Negócio 4 - Total de Vendas de Assinaturas do Minecraft Season Pass</t>
+  </si>
+  <si>
+    <t>Soma de Minecraft Season Pass Price</t>
   </si>
 </sst>
 </file>
@@ -1295,19 +1301,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1467,15 +1461,6 @@
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1520,8 +1505,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SlicerStyleLight6 2" pivot="0" table="0" count="10" xr9:uid="{14279B14-3B4E-4DF9-8110-D0080E74140C}">
-      <tableStyleElement type="wholeTable" dxfId="46"/>
-      <tableStyleElement type="headerRow" dxfId="45"/>
+      <tableStyleElement type="wholeTable" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="41"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1540,703 +1525,7 @@
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
-      <x14:dxfs count="32">
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.79998168889431442"/>
-              <bgColor theme="9" tint="0.79998168889431442"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.59999389629810485"/>
-              <bgColor theme="9" tint="0.59999389629810485"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFE0E0E0"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFE0E0E0"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFE0E0E0"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFE0E0E0"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.79998168889431442"/>
-              <bgColor theme="9" tint="0.79998168889431442"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.59999389629810485"/>
-              <bgColor theme="9" tint="0.59999389629810485"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFE0E0E0"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFE0E0E0"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFE0E0E0"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFE0E0E0"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.79998168889431442"/>
-              <bgColor theme="9" tint="0.79998168889431442"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="9" tint="0.59999389629810485"/>
-              <bgColor theme="9" tint="0.59999389629810485"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF828282"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFE0E0E0"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFE0E0E0"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFE0E0E0"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFE0E0E0"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFFFFFFF"/>
-              <bgColor rgb="FFFFFFFF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFCCCCCC"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFCCCCCC"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFCCCCCC"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFCCCCCC"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
+      <x14:dxfs count="8">
         <dxf>
           <font>
             <color rgb="FF000000"/>
@@ -4428,13 +3717,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>54871</xdr:rowOff>
+      <xdr:rowOff>44104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>309563</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>107156</xdr:rowOff>
+      <xdr:rowOff>96389</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4449,7 +3738,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2505489" y="1438067"/>
+          <a:off x="2505489" y="1427300"/>
           <a:ext cx="5026509" cy="1642546"/>
           <a:chOff x="2505489" y="1438067"/>
           <a:chExt cx="5026509" cy="1642546"/>
@@ -4679,6 +3968,322 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>612084</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>41154</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>321158</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>99339</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="Agrupar 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695DC36C-DC68-4DD9-9C14-D9AE687770EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7834519" y="1424350"/>
+          <a:ext cx="5026509" cy="1648446"/>
+          <a:chOff x="7834519" y="1416533"/>
+          <a:chExt cx="5026509" cy="1648446"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Retângulo: Cantos Arredondados 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4B848C-43E0-4DF7-9361-475A3FB64DCA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7834519" y="1421193"/>
+            <a:ext cx="5026508" cy="1637886"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 6990"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="C̳álculos!F41">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Retângulo: Cantos Arredondados 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD438E9-11E8-497F-A3B5-D741F84F99DD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9296499" y="1935128"/>
+            <a:ext cx="3427756" cy="1129851"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 6990"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:fld id="{8FD901DD-AFF6-4407-9156-ABB7C07BFC52}" type="TxLink">
+              <a:rPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="5BF6A8"/>
+                </a:solidFill>
+                <a:latin typeface="Aptos Narrow"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:t> R$ 1.800,00 </a:t>
+            </a:fld>
+            <a:endParaRPr lang="pt-BR" sz="3600" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="5BF6A8"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Retângulo: Cantos Superiores Arredondados 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEBEDF8-6A7F-4ADB-A347-09E0A3F84D39}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7834519" y="1416533"/>
+            <a:ext cx="5026509" cy="619643"/>
+          </a:xfrm>
+          <a:prstGeom prst="round2SameRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="2AE6B1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>TOTAL SUBSCRITIONS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> MINECRAFT SEASON PASS</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1100" b="1">
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="17" name="Agrupar 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D8BBE9B-DCEB-4F1C-8886-E263B28E7A27}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8083826" y="2150482"/>
+            <a:ext cx="1579294" cy="612913"/>
+            <a:chOff x="3495675" y="5400674"/>
+            <a:chExt cx="1549476" cy="752476"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="18" name="Imagem 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A44B7B7-C4F8-4171-80BD-5D0E1BFF7026}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3998608" y="5400674"/>
+              <a:ext cx="555497" cy="609599"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="19" name="Gráfico 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8507AD5-47DD-473C-86BD-0058BE8E76E9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+              <a:extLst>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3495675" y="5895937"/>
+              <a:ext cx="1549476" cy="257213"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9178,6 +8783,87 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E054BDCF-FE11-4FDB-B8E0-E10861C89C0F}" name="Tabela dinâmica3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="B37:C41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="6" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Soma de Minecraft Season Pass Price" fld="10" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7152702-2DC3-4B9B-BADD-D539D663B306}" name="Tbl_easeasonpass_total" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B24:C28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
@@ -9242,7 +8928,7 @@
     <dataField name="Soma de EA Play Season Pass" fld="8" baseField="2" baseItem="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="44">
+    <format dxfId="40">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9258,7 +8944,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EC8D6D2-BFCC-48E6-989A-4B46A9CE0253}" name="Tbl_annual_total" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B12:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
@@ -9313,32 +8999,11 @@
     <dataField name="Soma de Total Value" fld="12" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="50">
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
+  <chartFormats count="1">
     <chartFormat chart="3" format="3" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -9366,6 +9031,7 @@
   <pivotTables>
     <pivotTable tabId="3" name="Tbl_annual_total"/>
     <pivotTable tabId="3" name="Tbl_easeasonpass_total"/>
+    <pivotTable tabId="3" name="Tabela dinâmica3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1162036948">
@@ -9386,7 +9052,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="7">
       <filters>
@@ -9395,19 +9061,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="58" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="55" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="53" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="52" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="51" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="51" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="48" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="46" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="45" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="44" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -22079,16 +21745,16 @@
   <sheetPr>
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="B3:F28"/>
+  <dimension ref="B3:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.25" customWidth="1"/>
     <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
@@ -22218,12 +21884,69 @@
         <v>1350</v>
       </c>
     </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C37" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="15">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C41" s="15">
+        <v>1800</v>
+      </c>
+      <c r="F41" s="18">
+        <f>GETPIVOTDATA("Minecraft Season Pass Price",$B$37)</f>
+        <v>1800</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -22232,7 +21955,7 @@
   <dimension ref="A2:Q168"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Add icones e detalhes
</commit_message>
<xml_diff>
--- a/dashboard_xbox_sales.xlsx
+++ b/dashboard_xbox_sales.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DIO\DIO-Vendas-do-Xbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A27517D-E819-4421-8FBD-05B21A232711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA868F-F565-4961-A3D5-5653E9CEB520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="0" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
-    <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
-    <sheet name="B̳ases" sheetId="2" r:id="rId2"/>
-    <sheet name="C̳álculos" sheetId="3" r:id="rId3"/>
+    <sheet name="A̳ssets" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="B̳ases" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="C̳álculos" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="D̳ashboard" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -1262,7 +1262,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1294,6 +1294,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1301,121 +1304,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1502,8 +1391,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="SlicerStyleLight6 2" pivot="0" table="0" count="10" xr9:uid="{14279B14-3B4E-4DF9-8110-D0080E74140C}">
-      <tableStyleElement type="wholeTable" dxfId="41"/>
-      <tableStyleElement type="headerRow" dxfId="40"/>
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3525,15 +3414,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
+      <xdr:colOff>2090737</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>142873</xdr:rowOff>
+      <xdr:rowOff>152398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1262062</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>261936</xdr:rowOff>
+      <xdr:rowOff>271461</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3561,8 +3450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="547687" y="321467"/>
-          <a:ext cx="714375" cy="619125"/>
+          <a:off x="2090737" y="333373"/>
+          <a:ext cx="714375" cy="614363"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3907,14 +3796,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>612084</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>345384</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>41154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>321158</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>54458</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>99339</xdr:rowOff>
     </xdr:to>
@@ -3931,8 +3820,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7822509" y="1412754"/>
-          <a:ext cx="5014499" cy="1639335"/>
+          <a:off x="8241609" y="1412754"/>
+          <a:ext cx="5328824" cy="1639335"/>
           <a:chOff x="7834519" y="1416533"/>
           <a:chExt cx="5026509" cy="1648446"/>
         </a:xfrm>
@@ -4229,8 +4118,8 @@
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>331304</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
@@ -4248,7 +4137,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="2505076" y="3205161"/>
-          <a:ext cx="10342078" cy="3124201"/>
+          <a:ext cx="11077574" cy="3124201"/>
           <a:chOff x="2505490" y="3227110"/>
           <a:chExt cx="10365684" cy="3145322"/>
         </a:xfrm>
@@ -4420,6 +4309,225 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Elipse 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EC88DC-6099-4E0E-BBF5-26BADFEE12AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="514350" y="295275"/>
+          <a:ext cx="771525" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Retângulo 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13435013-DD35-4729-8D96-EFCC91F5BC8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="1028700"/>
+          <a:ext cx="1657350" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1">
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>&gt;Bem vindo, Julio</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>485775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Retângulo 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{583C6CAD-2C90-4706-AAE1-A7EDEAB3FFE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2457450" y="1162050"/>
+          <a:ext cx="6343650" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Calculation period: 01/01/2024 - 31/12/2024 | Update date: 13/04/2025 22:55:00</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8983,7 +9091,7 @@
     <dataField name="Soma de Minecraft Season Pass Price" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9064,7 +9172,7 @@
     <dataField name="Soma de EA Play Season Pass" fld="8" baseField="2" baseItem="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="39">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9135,7 +9243,7 @@
     <dataField name="Soma de Total Value" fld="12" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="42">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9188,7 +9296,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="18">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="7">
       <filters>
@@ -9197,19 +9305,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="50" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="48"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="47" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="45" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="44" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="43" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="12" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="9" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="7" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="6" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="5" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9538,7 +9646,7 @@
   <dimension ref="B3:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9711,7 +9819,7 @@
   <dimension ref="A1:M296"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:M294"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -22088,10 +22196,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
-  <dimension ref="A2:Q168"/>
+  <dimension ref="A2:R168"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="20" ySplit="35" topLeftCell="U36" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -22099,10 +22210,12 @@
     <col min="1" max="1" width="28" style="5" customWidth="1"/>
     <col min="2" max="2" width="3.625" customWidth="1"/>
     <col min="12" max="12" width="6.625" customWidth="1"/>
+    <col min="17" max="17" width="13.125" customWidth="1"/>
+    <col min="20" max="20" width="127" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="39" customHeight="1" thickBot="1">
-      <c r="C2" s="17" t="s">
+    <row r="2" spans="1:18" ht="39" customHeight="1" thickBot="1">
+      <c r="C2" s="19" t="s">
         <v>319</v>
       </c>
       <c r="D2" s="17"/>
@@ -22119,45 +22232,46 @@
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
-    </row>
-    <row r="3" spans="1:17" ht="39" customHeight="1" thickTop="1"/>
-    <row r="4" spans="1:17" s="7" customFormat="1" ht="8.25" customHeight="1">
+      <c r="R2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" ht="39" customHeight="1" thickTop="1"/>
+    <row r="4" spans="1:18" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:17" s="7" customFormat="1" ht="7.5" customHeight="1">
+    <row r="5" spans="1:18" s="7" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" ht="10.5" customHeight="1">
+    <row r="6" spans="1:18" s="7" customFormat="1" ht="10.5" customHeight="1">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" ht="9.75" customHeight="1">
+    <row r="7" spans="1:18" s="7" customFormat="1" ht="9.75" customHeight="1">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:17" s="7" customFormat="1" ht="33" customHeight="1">
+    <row r="8" spans="1:18" s="7" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:17" s="7" customFormat="1">
+    <row r="9" spans="1:18" s="7" customFormat="1">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:17" s="7" customFormat="1">
+    <row r="10" spans="1:18" s="7" customFormat="1">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:17" s="7" customFormat="1">
+    <row r="11" spans="1:18" s="7" customFormat="1">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:17" s="7" customFormat="1">
+    <row r="12" spans="1:18" s="7" customFormat="1">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:17" s="7" customFormat="1">
+    <row r="13" spans="1:18" s="7" customFormat="1">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:17" s="7" customFormat="1">
+    <row r="14" spans="1:18" s="7" customFormat="1">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:17" s="7" customFormat="1">
+    <row r="15" spans="1:18" s="7" customFormat="1">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:17" s="7" customFormat="1">
+    <row r="16" spans="1:18" s="7" customFormat="1">
       <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" s="7" customFormat="1">
@@ -22211,19 +22325,19 @@
     <row r="33" spans="1:1" s="7" customFormat="1">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" s="7" customFormat="1">
+    <row r="34" spans="1:1" s="7" customFormat="1" ht="83.25" customHeight="1">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" s="7" customFormat="1">
+    <row r="35" spans="1:1" s="7" customFormat="1" ht="75.75" customHeight="1">
       <c r="A35" s="5"/>
     </row>
     <row r="36" spans="1:1" s="7" customFormat="1">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" s="7" customFormat="1">
+    <row r="37" spans="1:1" s="7" customFormat="1" ht="38.25" customHeight="1">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" s="7" customFormat="1">
+    <row r="38" spans="1:1" s="7" customFormat="1" ht="33" customHeight="1">
       <c r="A38" s="5"/>
     </row>
     <row r="39" spans="1:1" s="7" customFormat="1">

</xml_diff>